<commit_message>
v1.1 convert using pyodide-worker
</commit_message>
<xml_diff>
--- a/data/starbound_data.xlsx
+++ b/data/starbound_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\campaign_dashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD2A09BF-20D0-4643-B736-676CF9F726E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{023944C8-25FA-4D17-BEE5-F942CE2BA664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{63028853-D2A9-47E4-8FD4-99117B4633E5}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="2" xr2:uid="{63028853-D2A9-47E4-8FD4-99117B4633E5}"/>
   </bookViews>
   <sheets>
     <sheet name="pc_rolls_overview" sheetId="2" r:id="rId1"/>
@@ -612,7 +612,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39166F29-CC4B-498B-AFD0-9B5550032F47}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
     </sheetView>
@@ -1093,9 +1093,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0DACA06-1040-464F-9CB0-D287674473A4}">
   <dimension ref="A1:H127"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A128" sqref="A128"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I64" sqref="I64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>